<commit_message>
parallel and headless code changes
</commit_message>
<xml_diff>
--- a/target/test-classes/Excels/NOVO_testcases_masterexcel.xlsx
+++ b/target/test-classes/Excels/NOVO_testcases_masterexcel.xlsx
@@ -169,9 +169,6 @@
     <t>SkillLevel</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Software Quality Assurance</t>
   </si>
   <si>
@@ -196,7 +193,10 @@
     <t>automationtest@pixentia.com</t>
   </si>
   <si>
-    <t>automation</t>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -722,7 +722,7 @@
         <v>40</v>
       </c>
       <c r="N1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -736,7 +736,7 @@
         <v>33</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
@@ -780,7 +780,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -829,28 +829,28 @@
         <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>56</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>47</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>48</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
         <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>